<commit_message>
Goods Receive module written
</commit_message>
<xml_diff>
--- a/resources/Goods/GoodsReceive/GoodsReceive.xlsx
+++ b/resources/Goods/GoodsReceive/GoodsReceive.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\win10\eclipse-workspace\FirstTestNG\resources\Goods\GoodsReceive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8BC9442-38CE-4F7E-BF3D-018931A4DC01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7010D07-C3C7-4E31-A8C0-94E8D5FBAB67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="60">
   <si>
     <t>SkuVariationName</t>
   </si>
@@ -169,6 +169,45 @@
   </si>
   <si>
     <t>SKU 10</t>
+  </si>
+  <si>
+    <t>NoOfItemsVariatoin</t>
+  </si>
+  <si>
+    <t>NoOfSKUforStockUpdation</t>
+  </si>
+  <si>
+    <t>Sno</t>
+  </si>
+  <si>
+    <t>update Stock</t>
+  </si>
+  <si>
+    <t>test SKU 302</t>
+  </si>
+  <si>
+    <t>test SKU 303</t>
+  </si>
+  <si>
+    <t>test SKU automation 3</t>
+  </si>
+  <si>
+    <t>test SKU automation 5</t>
+  </si>
+  <si>
+    <t>test SKU automation 8</t>
+  </si>
+  <si>
+    <t>test SKU automation 9</t>
+  </si>
+  <si>
+    <t>test SKU automation 6</t>
+  </si>
+  <si>
+    <t>test SKU automation 4</t>
+  </si>
+  <si>
+    <t>test SKU automation 7</t>
   </si>
 </sst>
 </file>
@@ -184,7 +223,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -209,8 +248,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -294,11 +339,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -314,8 +397,45 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -596,10 +716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M44"/>
+  <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,8 +741,8 @@
       <c r="A1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="4">
-        <v>1</v>
+      <c r="B1" s="14">
+        <v>3</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -633,6 +753,7 @@
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="9"/>
+      <c r="L1" s="25"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -666,7 +787,7 @@
       <c r="K2" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="L2" s="1"/>
+      <c r="L2" s="20"/>
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -676,8 +797,12 @@
       <c r="B3" s="5">
         <v>1245</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="C3" s="28">
+        <v>1245</v>
+      </c>
+      <c r="D3" s="28">
+        <v>1245</v>
+      </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
@@ -685,7 +810,7 @@
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="7"/>
-      <c r="L3" s="1"/>
+      <c r="L3" s="20"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -694,8 +819,12 @@
       <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
+      <c r="C4" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>52</v>
+      </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
@@ -703,7 +832,7 @@
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="7"/>
-      <c r="L4" s="1"/>
+      <c r="L4" s="20"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -712,8 +841,12 @@
       <c r="B5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
+      <c r="C5" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>32</v>
+      </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
@@ -721,7 +854,7 @@
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="7"/>
-      <c r="L5" s="1"/>
+      <c r="L5" s="20"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -730,8 +863,12 @@
       <c r="B6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
+      <c r="C6" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>30</v>
+      </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
@@ -739,17 +876,21 @@
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="7"/>
-      <c r="L6" s="1"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L6" s="20"/>
+    </row>
+    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
+      <c r="C7" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>28</v>
+      </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
@@ -757,7 +898,7 @@
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="7"/>
-      <c r="L7" s="1"/>
+      <c r="L7" s="20"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -766,8 +907,12 @@
       <c r="B8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+      <c r="C8" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>26</v>
+      </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
@@ -775,7 +920,7 @@
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="7"/>
-      <c r="L8" s="1"/>
+      <c r="L8" s="20"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -784,8 +929,12 @@
       <c r="B9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+      <c r="C9" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>23</v>
+      </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -793,7 +942,7 @@
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="7"/>
-      <c r="L9" s="1"/>
+      <c r="L9" s="20"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -802,8 +951,12 @@
       <c r="B10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
+      <c r="C10" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>23</v>
+      </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
@@ -811,7 +964,7 @@
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="7"/>
-      <c r="L10" s="1"/>
+      <c r="L10" s="20"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -820,8 +973,12 @@
       <c r="B11" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
+      <c r="C11" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>21</v>
+      </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
@@ -829,7 +986,7 @@
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="7"/>
-      <c r="L11" s="1"/>
+      <c r="L11" s="20"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
@@ -838,8 +995,12 @@
       <c r="B12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+      <c r="C12" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>19</v>
+      </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
@@ -847,33 +1008,43 @@
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="7"/>
-      <c r="L12" s="1"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="L12" s="20"/>
+    </row>
+    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
+      <c r="B13" s="15">
+        <v>2</v>
+      </c>
+      <c r="C13" s="29">
+        <v>3</v>
+      </c>
+      <c r="D13" s="29">
+        <v>4</v>
+      </c>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
       <c r="K13" s="7"/>
-      <c r="L13" s="1"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L13" s="20"/>
+    </row>
+    <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+      <c r="C14" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>57</v>
+      </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
@@ -881,7 +1052,7 @@
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="7"/>
-      <c r="L14" s="1"/>
+      <c r="L14" s="20"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
@@ -890,8 +1061,12 @@
       <c r="B15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
+      <c r="C15" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>17</v>
+      </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
@@ -899,7 +1074,7 @@
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="7"/>
-      <c r="L15" s="1"/>
+      <c r="L15" s="20"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -908,8 +1083,12 @@
       <c r="B16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
+      <c r="C16" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>16</v>
+      </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
@@ -917,17 +1096,21 @@
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="7"/>
-      <c r="L16" s="1"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L16" s="20"/>
+    </row>
+    <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
+      <c r="C17" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>59</v>
+      </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
@@ -935,7 +1118,7 @@
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="7"/>
-      <c r="L17" s="1"/>
+      <c r="L17" s="20"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
@@ -944,8 +1127,12 @@
       <c r="B18" s="5">
         <v>180</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
+      <c r="C18" s="28">
+        <v>180</v>
+      </c>
+      <c r="D18" s="28">
+        <v>180</v>
+      </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
@@ -953,7 +1140,7 @@
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="7"/>
-      <c r="L18" s="1"/>
+      <c r="L18" s="20"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
@@ -962,8 +1149,12 @@
       <c r="B19" s="5">
         <v>3</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
+      <c r="C19" s="28">
+        <v>3</v>
+      </c>
+      <c r="D19" s="28">
+        <v>3</v>
+      </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
@@ -971,15 +1162,19 @@
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="7"/>
-      <c r="L19" s="1"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L19" s="20"/>
+    </row>
+    <row r="20" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
+      <c r="C20" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>55</v>
+      </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
@@ -987,15 +1182,19 @@
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="7"/>
-      <c r="L20" s="1"/>
+      <c r="L20" s="20"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
+      <c r="C21" s="28">
+        <v>200</v>
+      </c>
+      <c r="D21" s="28">
+        <v>200</v>
+      </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
@@ -1003,15 +1202,19 @@
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
       <c r="K21" s="7"/>
-      <c r="L21" s="1"/>
+      <c r="L21" s="20"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
+      <c r="C22" s="28">
+        <v>0.5</v>
+      </c>
+      <c r="D22" s="28">
+        <v>0.5</v>
+      </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
@@ -1019,15 +1222,17 @@
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="7"/>
-      <c r="L22" s="1"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L22" s="20"/>
+    </row>
+    <row r="23" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18" t="s">
+        <v>56</v>
+      </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
@@ -1035,15 +1240,17 @@
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
       <c r="K23" s="7"/>
-      <c r="L23" s="1"/>
+      <c r="L23" s="20"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="28">
+        <v>200</v>
+      </c>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
@@ -1051,15 +1258,17 @@
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
       <c r="K24" s="7"/>
-      <c r="L24" s="1"/>
+      <c r="L24" s="20"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>13</v>
       </c>
       <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="28">
+        <v>0.5</v>
+      </c>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
@@ -1067,9 +1276,21 @@
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
       <c r="K25" s="10"/>
-      <c r="L25" s="1"/>
-    </row>
-    <row r="26" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="L25" s="20"/>
+    </row>
+    <row r="26" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="22"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="21"/>
+      <c r="K26" s="21"/>
+    </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>4</v>
@@ -1077,163 +1298,342 @@
       <c r="B27" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="14"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="7"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="10"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="C29" s="20"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+    </row>
+    <row r="30" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="17">
+        <v>6</v>
+      </c>
+      <c r="C30" s="20"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+    </row>
+    <row r="31" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" s="17">
         <v>3</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C31" s="23"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="D32" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="E32" s="19" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
+      <c r="F32" s="25"/>
+      <c r="G32" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="H32" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="I32" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="18">
+        <v>1</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="C33" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="4">
+      <c r="D33" s="4">
         <v>5</v>
       </c>
-      <c r="D31" s="7">
+      <c r="E33" s="7">
         <v>20</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
+      <c r="F33" s="25"/>
+      <c r="G33" s="18">
+        <v>1</v>
+      </c>
+      <c r="H33" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="I33" s="18">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="18">
+        <v>2</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="4">
+      <c r="D34" s="4">
         <v>6</v>
       </c>
-      <c r="D32" s="7">
+      <c r="E34" s="7">
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="7"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="7"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="7"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="7"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="7"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="7"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="18">
+        <v>2</v>
+      </c>
+      <c r="H34" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="I34" s="18">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="18">
+        <v>3</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D35" s="26">
+        <v>7</v>
+      </c>
+      <c r="E35" s="7">
+        <v>40</v>
+      </c>
+      <c r="F35" s="25"/>
+      <c r="G35" s="18">
+        <v>3</v>
+      </c>
+      <c r="H35" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="I35" s="18">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="18">
+        <v>4</v>
+      </c>
+      <c r="B36" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D36" s="26">
+        <v>8</v>
+      </c>
+      <c r="E36" s="7">
+        <v>50</v>
+      </c>
+      <c r="F36" s="25"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="18"/>
+    </row>
+    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="18">
+        <v>5</v>
+      </c>
+      <c r="B37" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D37" s="26">
+        <v>7</v>
+      </c>
+      <c r="E37" s="7">
+        <v>60</v>
+      </c>
+      <c r="F37" s="25"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="18"/>
+    </row>
+    <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="18">
+        <v>6</v>
+      </c>
+      <c r="B38" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D38" s="26">
+        <v>8</v>
+      </c>
+      <c r="E38" s="7">
+        <v>70</v>
+      </c>
+      <c r="F38" s="25"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="18"/>
+      <c r="I38" s="18"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="18"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
-      <c r="D39" s="7"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="25"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="18"/>
+      <c r="I39" s="18"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="18"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
-      <c r="D40" s="7"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="25"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="18"/>
+      <c r="I40" s="18"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="18"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
-      <c r="D41" s="7"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="25"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="18"/>
+      <c r="I41" s="18"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="18"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
-      <c r="D42" s="7"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="25"/>
+      <c r="G42" s="18"/>
+      <c r="H42" s="18"/>
+      <c r="I42" s="18"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="18"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
-      <c r="D43" s="7"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="25"/>
+      <c r="G43" s="18"/>
+      <c r="H43" s="18"/>
+      <c r="I43" s="18"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="18"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
-      <c r="D44" s="7"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="25"/>
+      <c r="G44" s="18"/>
+      <c r="H44" s="18"/>
+      <c r="I44" s="18"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="18"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="25"/>
+      <c r="G45" s="18"/>
+      <c r="H45" s="18"/>
+      <c r="I45" s="18"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="18"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="25"/>
+      <c r="G46" s="18"/>
+      <c r="H46" s="18"/>
+      <c r="I46" s="18"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>